<commit_message>
changed loom to youtube
</commit_message>
<xml_diff>
--- a/144F20/Topic 1/QR_5-1_Tech_Template.xlsx
+++ b/144F20/Topic 1/QR_5-1_Tech_Template.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\richard.ketchersid\OneDrive - GCU Employees\Course Materials\git\Teaching\144F20\Topic 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gcumail-my.sharepoint.com/personal/richard_ketchersid_gcu_edu/Documents/Course Materials/git/Teaching/144F20/Topic 1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:80_{5923E150-398C-4435-B211-D4FA3DC7DB09}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:80_{A91F6560-5637-4517-894C-73D0B2316A03}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="885" yWindow="555" windowWidth="21795" windowHeight="13530" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="885" yWindow="555" windowWidth="19335" windowHeight="13605" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
   <customWorkbookViews>
-    <customWorkbookView name="Richard Ketchersid - Personal View" guid="{B62E1535-74BF-4942-B420-625B8B4ACDDA}" mergeInterval="0" personalView="1" xWindow="59" yWindow="37" windowWidth="1453" windowHeight="902" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Richard Ketchersid - Personal View" guid="{B62E1535-74BF-4942-B420-625B8B4ACDDA}" mergeInterval="0" personalView="1" xWindow="59" yWindow="37" windowWidth="1289" windowHeight="907" tabRatio="500" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -633,9 +633,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -682,6 +679,75 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -690,61 +756,11 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -761,25 +777,9 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -822,8 +822,8 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{07306E0B-6D2B-4C08-A858-D10090994BD5}">
-  <header guid="{07306E0B-6D2B-4C08-A858-D10090994BD5}" dateTime="2021-04-23T13:21:36" maxSheetId="2" userName="Richard Ketchersid" r:id="rId1">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{8DB5CF34-9561-4DF0-884C-ABAF59410CE8}">
+  <header guid="{8DB5CF34-9561-4DF0-884C-ABAF59410CE8}" dateTime="2022-03-17T23:04:41" maxSheetId="2" userName="Richard Ketchersid" r:id="rId1">
     <sheetIdMap count="1">
       <sheetId val="1"/>
     </sheetIdMap>
@@ -837,7 +837,7 @@
 
 <file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
 <users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="1">
-  <userInfo guid="{07306E0B-6D2B-4C08-A858-D10090994BD5}" name="Richard Ketchersid" id="-1739574577" dateTime="2021-04-23T13:21:36"/>
+  <userInfo guid="{8DB5CF34-9561-4DF0-884C-ABAF59410CE8}" name="Richard Ketchersid" id="-1739585400" dateTime="2022-03-17T23:04:41"/>
 </users>
 </file>
 
@@ -1166,7 +1166,7 @@
   <dimension ref="A1:K42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E2" sqref="E2:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1183,53 +1183,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="16"/>
-      <c r="B1" s="17"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
+      <c r="A1" s="15"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
     </row>
     <row r="2" spans="1:11" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="50" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="47" t="s">
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="53" t="s">
         <v>33</v>
       </c>
-      <c r="F2" s="48"/>
-      <c r="G2" s="20"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="19"/>
     </row>
     <row r="3" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="18"/>
-      <c r="B3" s="19"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
+      <c r="A3" s="17"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
     </row>
     <row r="4" spans="1:11" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="53" t="s">
+      <c r="B4" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="53"/>
-      <c r="D4" s="54" t="s">
+      <c r="C4" s="49"/>
+      <c r="D4" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="54"/>
-      <c r="F4" s="55"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="26" t="s">
+      <c r="E4" s="55"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="I4" s="27"/>
-      <c r="J4" s="16"/>
+      <c r="I4" s="47"/>
+      <c r="J4" s="15"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
@@ -1241,465 +1241,467 @@
       <c r="D5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="21" t="s">
+      <c r="E5" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="H5" s="28" t="s">
+      <c r="H5" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="I5" s="29" t="s">
+      <c r="I5" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="K5" s="20"/>
+      <c r="K5" s="19"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="49" t="s">
+      <c r="A6" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="50"/>
-      <c r="C6" s="50"/>
-      <c r="D6" s="50"/>
-      <c r="E6" s="51"/>
-      <c r="H6" s="30" t="s">
+      <c r="B6" s="35"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="36"/>
+      <c r="H6" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="I6" s="31" t="s">
+      <c r="I6" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="K6" s="20"/>
+      <c r="K6" s="19"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="22"/>
-      <c r="H7" s="32" t="s">
+      <c r="B7" s="5"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="21"/>
+      <c r="H7" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="I7" s="31" t="s">
+      <c r="I7" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="K7" s="20"/>
+      <c r="K7" s="19"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="24"/>
-      <c r="H8" s="33" t="s">
+      <c r="B8" s="7"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="23"/>
+      <c r="H8" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="I8" s="31" t="s">
+      <c r="I8" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="K8" s="20"/>
+      <c r="K8" s="19"/>
     </row>
     <row r="9" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="24"/>
-      <c r="H9" s="34" t="s">
+      <c r="B9" s="7"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="23"/>
+      <c r="H9" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="I9" s="35" t="s">
+      <c r="I9" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="K9" s="20"/>
+      <c r="K9" s="19"/>
     </row>
     <row r="10" spans="1:11" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="24"/>
-      <c r="K10" s="20"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="23"/>
+      <c r="K10" s="19"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="23"/>
-      <c r="K11" s="20"/>
+      <c r="A11" s="10"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="22"/>
+      <c r="K11" s="19"/>
     </row>
     <row r="12" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="49" t="s">
+      <c r="A12" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="50"/>
-      <c r="C12" s="50"/>
-      <c r="D12" s="50"/>
-      <c r="E12" s="51"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="16"/>
-      <c r="J12" s="16"/>
-      <c r="K12" s="20"/>
+      <c r="B12" s="35"/>
+      <c r="C12" s="35"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="19"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="6"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="36" t="s">
+      <c r="B13" s="5"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="G13" s="37"/>
-      <c r="H13" s="37"/>
-      <c r="I13" s="37"/>
-      <c r="J13" s="38"/>
-      <c r="K13" s="20"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="38"/>
+      <c r="I13" s="38"/>
+      <c r="J13" s="39"/>
+      <c r="K13" s="19"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="8"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="39"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="40"/>
-      <c r="K14" s="20"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="41"/>
+      <c r="H14" s="41"/>
+      <c r="I14" s="41"/>
+      <c r="J14" s="42"/>
+      <c r="K14" s="19"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="8"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="39"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="40"/>
-      <c r="K15" s="20"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="40"/>
+      <c r="G15" s="41"/>
+      <c r="H15" s="41"/>
+      <c r="I15" s="41"/>
+      <c r="J15" s="42"/>
+      <c r="K15" s="19"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="8"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="39"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="40"/>
-      <c r="K16" s="20"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="40"/>
+      <c r="G16" s="41"/>
+      <c r="H16" s="41"/>
+      <c r="I16" s="41"/>
+      <c r="J16" s="42"/>
+      <c r="K16" s="19"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="11"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="23"/>
-      <c r="F17" s="39"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="40"/>
-      <c r="K17" s="20"/>
+      <c r="A17" s="10"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="41"/>
+      <c r="H17" s="41"/>
+      <c r="I17" s="41"/>
+      <c r="J17" s="42"/>
+      <c r="K17" s="19"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="49" t="s">
+      <c r="A18" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="B18" s="50"/>
-      <c r="C18" s="50"/>
-      <c r="D18" s="50"/>
-      <c r="E18" s="52"/>
-      <c r="F18" s="39"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="40"/>
-      <c r="K18" s="20"/>
+      <c r="B18" s="35"/>
+      <c r="C18" s="35"/>
+      <c r="D18" s="35"/>
+      <c r="E18" s="48"/>
+      <c r="F18" s="40"/>
+      <c r="G18" s="41"/>
+      <c r="H18" s="41"/>
+      <c r="I18" s="41"/>
+      <c r="J18" s="42"/>
+      <c r="K18" s="19"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B19" s="6"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="22"/>
-      <c r="F19" s="39"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="40"/>
-      <c r="K19" s="20"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="40"/>
+      <c r="G19" s="41"/>
+      <c r="H19" s="41"/>
+      <c r="I19" s="41"/>
+      <c r="J19" s="42"/>
+      <c r="K19" s="19"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B20" s="8"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="24"/>
-      <c r="F20" s="39"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="40"/>
-      <c r="K20" s="20"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="40"/>
+      <c r="G20" s="41"/>
+      <c r="H20" s="41"/>
+      <c r="I20" s="41"/>
+      <c r="J20" s="42"/>
+      <c r="K20" s="19"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B21" s="8"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="24"/>
-      <c r="F21" s="39"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="40"/>
-      <c r="K21" s="20"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="23"/>
+      <c r="F21" s="40"/>
+      <c r="G21" s="41"/>
+      <c r="H21" s="41"/>
+      <c r="I21" s="41"/>
+      <c r="J21" s="42"/>
+      <c r="K21" s="19"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B22" s="8"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="24"/>
-      <c r="F22" s="39"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
-      <c r="J22" s="40"/>
-      <c r="K22" s="20"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="23"/>
+      <c r="F22" s="40"/>
+      <c r="G22" s="41"/>
+      <c r="H22" s="41"/>
+      <c r="I22" s="41"/>
+      <c r="J22" s="42"/>
+      <c r="K22" s="19"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="11"/>
-      <c r="B23" s="12"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="23"/>
-      <c r="F23" s="39"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
-      <c r="J23" s="40"/>
-      <c r="K23" s="20"/>
+      <c r="A23" s="10"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="22"/>
+      <c r="F23" s="40"/>
+      <c r="G23" s="41"/>
+      <c r="H23" s="41"/>
+      <c r="I23" s="41"/>
+      <c r="J23" s="42"/>
+      <c r="K23" s="19"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="49" t="s">
+      <c r="A24" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="B24" s="50"/>
-      <c r="C24" s="50"/>
-      <c r="D24" s="50"/>
-      <c r="E24" s="52"/>
-      <c r="F24" s="39"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="5"/>
-      <c r="J24" s="40"/>
-      <c r="K24" s="20"/>
+      <c r="B24" s="35"/>
+      <c r="C24" s="35"/>
+      <c r="D24" s="35"/>
+      <c r="E24" s="48"/>
+      <c r="F24" s="40"/>
+      <c r="G24" s="41"/>
+      <c r="H24" s="41"/>
+      <c r="I24" s="41"/>
+      <c r="J24" s="42"/>
+      <c r="K24" s="19"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="22"/>
-      <c r="F25" s="39"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="5"/>
-      <c r="J25" s="40"/>
-      <c r="K25" s="20"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="21"/>
+      <c r="F25" s="40"/>
+      <c r="G25" s="41"/>
+      <c r="H25" s="41"/>
+      <c r="I25" s="41"/>
+      <c r="J25" s="42"/>
+      <c r="K25" s="19"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B26" s="8"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="24"/>
-      <c r="F26" s="39"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="5"/>
-      <c r="I26" s="5"/>
-      <c r="J26" s="40"/>
-      <c r="K26" s="20"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="23"/>
+      <c r="F26" s="40"/>
+      <c r="G26" s="41"/>
+      <c r="H26" s="41"/>
+      <c r="I26" s="41"/>
+      <c r="J26" s="42"/>
+      <c r="K26" s="19"/>
     </row>
     <row r="27" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B27" s="8"/>
-      <c r="C27" s="9"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="41"/>
-      <c r="G27" s="42"/>
-      <c r="H27" s="42"/>
-      <c r="I27" s="42"/>
-      <c r="J27" s="43"/>
-      <c r="K27" s="20"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="23"/>
+      <c r="F27" s="43"/>
+      <c r="G27" s="44"/>
+      <c r="H27" s="44"/>
+      <c r="I27" s="44"/>
+      <c r="J27" s="45"/>
+      <c r="K27" s="19"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B28" s="8"/>
-      <c r="C28" s="9"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="18"/>
-      <c r="H28" s="18"/>
-      <c r="I28" s="18"/>
-      <c r="J28" s="18"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="17"/>
+      <c r="G28" s="17"/>
+      <c r="H28" s="17"/>
+      <c r="I28" s="17"/>
+      <c r="J28" s="17"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="11"/>
-      <c r="B29" s="12"/>
-      <c r="C29" s="13"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="14"/>
+      <c r="A29" s="10"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="49" t="s">
+      <c r="A30" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="B30" s="50"/>
-      <c r="C30" s="50"/>
-      <c r="D30" s="50"/>
-      <c r="E30" s="51"/>
+      <c r="B30" s="35"/>
+      <c r="C30" s="35"/>
+      <c r="D30" s="35"/>
+      <c r="E30" s="36"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
-      <c r="B31" s="6"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="15"/>
-      <c r="E31" s="7"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="6"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B32" s="8"/>
-      <c r="C32" s="9"/>
-      <c r="D32" s="10"/>
-      <c r="E32" s="25"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="24"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B33" s="8"/>
-      <c r="C33" s="9"/>
-      <c r="D33" s="10"/>
-      <c r="E33" s="25"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="24"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B34" s="8"/>
-      <c r="C34" s="9"/>
-      <c r="D34" s="10"/>
-      <c r="E34" s="25"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="24"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="11"/>
-      <c r="B35" s="12"/>
-      <c r="C35" s="13"/>
-      <c r="D35" s="14"/>
-      <c r="E35" s="14"/>
+      <c r="A35" s="10"/>
+      <c r="B35" s="11"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="49" t="s">
+      <c r="A36" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="B36" s="50"/>
-      <c r="C36" s="50"/>
-      <c r="D36" s="50"/>
-      <c r="E36" s="51"/>
+      <c r="B36" s="35"/>
+      <c r="C36" s="35"/>
+      <c r="D36" s="35"/>
+      <c r="E36" s="36"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B37" s="6"/>
-      <c r="C37" s="7"/>
-      <c r="D37" s="15"/>
-      <c r="E37" s="7"/>
+      <c r="B37" s="5"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="14"/>
+      <c r="E37" s="6"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B38" s="8"/>
-      <c r="C38" s="9"/>
-      <c r="D38" s="10"/>
-      <c r="E38" s="25"/>
+      <c r="B38" s="7"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="24"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B39" s="8"/>
-      <c r="C39" s="9"/>
-      <c r="D39" s="10"/>
-      <c r="E39" s="25"/>
+      <c r="B39" s="7"/>
+      <c r="C39" s="8"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="24"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B40" s="8"/>
-      <c r="C40" s="9"/>
-      <c r="D40" s="10"/>
-      <c r="E40" s="25"/>
+      <c r="B40" s="7"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="24"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B41" s="8"/>
-      <c r="C41" s="9"/>
-      <c r="D41" s="10"/>
-      <c r="E41" s="25"/>
+      <c r="B41" s="7"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="24"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="11"/>
-      <c r="B42" s="12"/>
-      <c r="C42" s="13"/>
-      <c r="D42" s="14"/>
-      <c r="E42" s="14"/>
+      <c r="A42" s="10"/>
+      <c r="B42" s="11"/>
+      <c r="C42" s="12"/>
+      <c r="D42" s="13"/>
+      <c r="E42" s="13"/>
     </row>
   </sheetData>
   <customSheetViews>
     <customSheetView guid="{B62E1535-74BF-4942-B420-625B8B4ACDDA}">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E2" sqref="E2:F2"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="12">
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="E2:F2"/>
     <mergeCell ref="A30:E30"/>
     <mergeCell ref="A36:E36"/>
     <mergeCell ref="F13:J27"/>
@@ -1710,8 +1712,6 @@
     <mergeCell ref="A24:E24"/>
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="B4:C4"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="E2:F2"/>
   </mergeCells>
   <conditionalFormatting sqref="A3:J42">
     <cfRule type="expression" dxfId="1" priority="2">
@@ -1726,9 +1726,10 @@
   <hyperlinks>
     <hyperlink ref="D4" r:id="rId2" display="Video" xr:uid="{4C1A7EA5-AB92-44B8-B05B-0A63318B4C1F}"/>
     <hyperlink ref="B4:C4" r:id="rId3" display="Video" xr:uid="{FF61B875-203B-4521-9C84-14017D0EBEB4}"/>
+    <hyperlink ref="D4:E4" r:id="rId4" display="Video (autofill)" xr:uid="{ADC89870-6C98-478F-9EE4-27DCEC7806D8}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>